<commit_message>
added code chunk for c14 dates
</commit_message>
<xml_diff>
--- a/analysis/data/raw_data/KWL_C14_dates.xlsx
+++ b/analysis/data/raw_data/KWL_C14_dates.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/EmilyWang/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/EmilyWang/Desktop/School document/LW-Paper/kwl-ornaments-2019/analysis/data/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6D258B3-6CC7-574E-8559-024F4B1F9B26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{348AE14E-C6D6-0340-A2DD-E36777EA7356}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3300" yWindow="460" windowWidth="15500" windowHeight="16060" xr2:uid="{8DD15795-9B77-D142-AB16-8DEEBD71ECC9}"/>
+    <workbookView xWindow="9100" yWindow="460" windowWidth="15500" windowHeight="16060" xr2:uid="{8DD15795-9B77-D142-AB16-8DEEBD71ECC9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="50">
   <si>
     <t>P041</t>
   </si>
@@ -164,16 +164,25 @@
     <t>Depth2</t>
   </si>
   <si>
-    <t>P049</t>
-  </si>
-  <si>
-    <t>340 ± 30</t>
-  </si>
-  <si>
-    <t>466 - 315</t>
-  </si>
-  <si>
     <t>279 - 0</t>
+  </si>
+  <si>
+    <t>period</t>
+  </si>
+  <si>
+    <t>pre-European</t>
+  </si>
+  <si>
+    <t>post-European</t>
+  </si>
+  <si>
+    <t>European</t>
+  </si>
+  <si>
+    <t>rce</t>
+  </si>
+  <si>
+    <t>se</t>
   </si>
 </sst>
 </file>
@@ -532,10 +541,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C44DE8E0-CB48-C741-8CBC-BBB68EC49E9D}">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -544,13 +553,12 @@
     <col min="2" max="2" width="7" customWidth="1"/>
     <col min="3" max="3" width="9.1640625" customWidth="1"/>
     <col min="4" max="4" width="8" customWidth="1"/>
-    <col min="6" max="6" width="14.83203125" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" customWidth="1"/>
-    <col min="8" max="8" width="6.33203125" customWidth="1"/>
+    <col min="6" max="7" width="14.83203125" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" customWidth="1"/>
     <col min="9" max="9" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
@@ -572,9 +580,17 @@
       <c r="G1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="1"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -594,9 +610,17 @@
         <v>28</v>
       </c>
       <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I2" s="1">
+        <v>250</v>
+      </c>
+      <c r="J2" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -616,9 +640,17 @@
         <v>30</v>
       </c>
       <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I3" s="1">
+        <v>900</v>
+      </c>
+      <c r="J3" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -638,293 +670,357 @@
         <v>31</v>
       </c>
       <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I4" s="1">
+        <v>1240</v>
+      </c>
+      <c r="J4" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>43</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="1">
-        <v>-20</v>
+        <v>0</v>
       </c>
       <c r="D5" s="1">
-        <v>-30</v>
+        <v>-40</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C6" s="1">
-        <v>0</v>
+        <v>-36</v>
       </c>
       <c r="D6" s="1">
-        <v>-40</v>
+        <v>-56</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H6" s="1"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J6" s="1"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C7" s="1">
-        <v>-36</v>
+        <v>-70</v>
       </c>
       <c r="D7" s="1">
-        <v>-56</v>
+        <v>-90</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C8" s="1">
-        <v>-70</v>
+        <v>0</v>
       </c>
       <c r="D8" s="1">
-        <v>-90</v>
+        <v>-40</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F8" s="1"/>
+      <c r="G8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J8" s="1"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C9" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D9" s="1">
-        <v>-40</v>
+        <v>-56</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F9" s="1"/>
+        <v>33</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="G9" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H9" s="1"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I9" s="1">
+        <v>510</v>
+      </c>
+      <c r="J9" s="1">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="C10" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D10" s="1">
-        <v>-56</v>
+        <v>-10</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H10" s="1"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J10" s="1"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="1">
+        <v>-110</v>
+      </c>
+      <c r="D11" s="1">
+        <v>-130</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I11" s="1">
+        <v>310</v>
+      </c>
+      <c r="J11" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="1">
+        <v>-10</v>
+      </c>
+      <c r="D12" s="1">
+        <v>-30</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J12" s="1"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="1">
+        <v>-40</v>
+      </c>
+      <c r="D13" s="1">
+        <v>-60</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I13" s="1">
+        <v>600</v>
+      </c>
+      <c r="J13" s="1">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="1">
+        <v>20</v>
+      </c>
+      <c r="D14" s="1">
+        <v>-57</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J14" s="1"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="1">
-        <v>0</v>
-      </c>
-      <c r="D11" s="1">
-        <v>-10</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F11" s="1" t="s">
+      <c r="C15" s="1">
+        <v>-20</v>
+      </c>
+      <c r="D15" s="1">
+        <v>-30</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="1">
-        <v>-110</v>
-      </c>
-      <c r="D12" s="1">
-        <v>-130</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C13" s="1">
-        <v>-10</v>
-      </c>
-      <c r="D13" s="1">
-        <v>-30</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H13" s="1"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="1">
-        <v>-40</v>
-      </c>
-      <c r="D14" s="1">
-        <v>-60</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" s="1">
-        <v>20</v>
-      </c>
-      <c r="D15" s="1">
-        <v>-57</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H15" s="1"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J15" s="1"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C16" s="1">
-        <v>-20</v>
+        <v>-50</v>
       </c>
       <c r="D16" s="1">
-        <v>-30</v>
+        <v>-70</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C17" s="1">
-        <v>-50</v>
-      </c>
-      <c r="D17" s="1">
-        <v>-70</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H16" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J16" s="1"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -933,7 +1029,7 @@
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>

</xml_diff>

<commit_message>
edited the text and revised the table
</commit_message>
<xml_diff>
--- a/analysis/data/raw_data/KWL_C14_dates.xlsx
+++ b/analysis/data/raw_data/KWL_C14_dates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/EmilyWang/Desktop/School document/LW-Paper/kwl-ornaments-2019/analysis/data/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{348AE14E-C6D6-0340-A2DD-E36777EA7356}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F07E7E77-8BF1-C447-836C-079C4216CC32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9100" yWindow="460" windowWidth="15500" windowHeight="16060" xr2:uid="{8DD15795-9B77-D142-AB16-8DEEBD71ECC9}"/>
+    <workbookView xWindow="320" yWindow="460" windowWidth="15500" windowHeight="16060" xr2:uid="{8DD15795-9B77-D142-AB16-8DEEBD71ECC9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -167,9 +167,6 @@
     <t>279 - 0</t>
   </si>
   <si>
-    <t>period</t>
-  </si>
-  <si>
     <t>pre-European</t>
   </si>
   <si>
@@ -183,6 +180,9 @@
   </si>
   <si>
     <t>se</t>
+  </si>
+  <si>
+    <t>Period</t>
   </si>
 </sst>
 </file>
@@ -544,7 +544,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -581,13 +581,13 @@
         <v>18</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -611,7 +611,7 @@
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I2" s="1">
         <v>250</v>
@@ -641,7 +641,7 @@
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I3" s="1">
         <v>900</v>
@@ -671,7 +671,7 @@
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I4" s="1">
         <v>1240</v>
@@ -701,7 +701,7 @@
         <v>19</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>5</v>
@@ -729,7 +729,7 @@
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>5</v>
@@ -757,7 +757,7 @@
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>5</v>
@@ -785,7 +785,7 @@
         <v>19</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>5</v>
@@ -815,7 +815,7 @@
         <v>20</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I9" s="1">
         <v>510</v>
@@ -845,7 +845,7 @@
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>5</v>
@@ -873,7 +873,7 @@
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I11" s="1">
         <v>310</v>
@@ -903,7 +903,7 @@
         <v>21</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>5</v>
@@ -931,7 +931,7 @@
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I13" s="1">
         <v>600</v>
@@ -961,7 +961,7 @@
         <v>22</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>5</v>
@@ -987,7 +987,7 @@
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>5</v>
@@ -1013,7 +1013,7 @@
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
added code for calibrated dates and created a new data file
</commit_message>
<xml_diff>
--- a/analysis/data/raw_data/KWL_C14_dates.xlsx
+++ b/analysis/data/raw_data/KWL_C14_dates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/EmilyWang/Desktop/School document/LW-Paper/kwl-ornaments-2019/analysis/data/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F07E7E77-8BF1-C447-836C-079C4216CC32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE88F837-17B9-104B-9D30-9E692A2F0E9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="460" windowWidth="15500" windowHeight="16060" xr2:uid="{8DD15795-9B77-D142-AB16-8DEEBD71ECC9}"/>
+    <workbookView xWindow="320" yWindow="460" windowWidth="17580" windowHeight="16060" xr2:uid="{8DD15795-9B77-D142-AB16-8DEEBD71ECC9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -92,18 +92,6 @@
     <t>Details</t>
   </si>
   <si>
-    <t>Midden, H026</t>
-  </si>
-  <si>
-    <t>Burial, M009</t>
-  </si>
-  <si>
-    <t>Midden, H032</t>
-  </si>
-  <si>
-    <t>burial, M095</t>
-  </si>
-  <si>
     <t>Square</t>
   </si>
   <si>
@@ -183,6 +171,18 @@
   </si>
   <si>
     <t>Period</t>
+  </si>
+  <si>
+    <t>Midden 26</t>
+  </si>
+  <si>
+    <t>Burial 9</t>
+  </si>
+  <si>
+    <t>Midden 32</t>
+  </si>
+  <si>
+    <t>Burial 95</t>
   </si>
 </sst>
 </file>
@@ -544,7 +544,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -560,34 +560,34 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>18</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -604,14 +604,14 @@
         <v>-45</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="I2" s="1">
         <v>250</v>
@@ -634,14 +634,14 @@
         <v>-90</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="I3" s="1">
         <v>900</v>
@@ -664,14 +664,14 @@
         <v>-170</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="I4" s="1">
         <v>1240</v>
@@ -698,10 +698,10 @@
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>5</v>
@@ -725,11 +725,11 @@
         <v>5</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>5</v>
@@ -753,11 +753,11 @@
         <v>5</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>5</v>
@@ -782,10 +782,10 @@
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>5</v>
@@ -806,16 +806,16 @@
         <v>-56</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="I9" s="1">
         <v>510</v>
@@ -841,11 +841,11 @@
         <v>5</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>5</v>
@@ -866,14 +866,14 @@
         <v>-130</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="I11" s="1">
         <v>310</v>
@@ -900,10 +900,10 @@
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>5</v>
@@ -924,14 +924,14 @@
         <v>-60</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="I13" s="1">
         <v>600</v>
@@ -958,10 +958,10 @@
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1" t="s">
-        <v>22</v>
+        <v>49</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>5</v>
@@ -987,7 +987,7 @@
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>5</v>
@@ -1013,7 +1013,7 @@
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
adjust the heading in the table and edit the figure caption
</commit_message>
<xml_diff>
--- a/analysis/data/raw_data/KWL_C14_dates.xlsx
+++ b/analysis/data/raw_data/KWL_C14_dates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/EmilyWang/Desktop/School document/LW-Paper/kwl-ornaments-2019/analysis/data/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{251C1998-434D-694D-9987-B40428EE4344}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A65D2164-ABEB-AD42-A7AB-C9A1188FE8E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="700" yWindow="460" windowWidth="22680" windowHeight="16540" xr2:uid="{8DD15795-9B77-D142-AB16-8DEEBD71ECC9}"/>
   </bookViews>
@@ -359,6 +359,9 @@
     <t>midden 26</t>
   </si>
   <si>
+    <t>midden 172</t>
+  </si>
+  <si>
     <t>burial 66</t>
   </si>
   <si>
@@ -372,9 +375,6 @@
   </si>
   <si>
     <t>burial 95</t>
-  </si>
-  <si>
-    <t>midden H172</t>
   </si>
   <si>
     <t>P018</t>
@@ -750,7 +750,7 @@
   <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1033,7 +1033,7 @@
         <v>40</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="I10" s="1">
         <v>270</v>
@@ -1085,7 +1085,7 @@
         <v>45</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="I12" s="1">
         <v>510</v>
@@ -1189,7 +1189,7 @@
         <v>48</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="I16" s="1">
         <v>360</v>
@@ -1276,7 +1276,7 @@
         <v>57</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="I19" s="1">
         <v>1190</v>
@@ -1415,7 +1415,7 @@
         <v>28</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="25" spans="1:10" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
@@ -1438,7 +1438,7 @@
         <v>71</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="I25" s="1">
         <v>280</v>

</xml_diff>

<commit_message>
edit the data file, work on the code for table, get an error
</commit_message>
<xml_diff>
--- a/analysis/data/raw_data/KWL_C14_dates.xlsx
+++ b/analysis/data/raw_data/KWL_C14_dates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/EmilyWang/Desktop/School document/LW-Paper/kwl-ornaments-2019/analysis/data/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A65D2164-ABEB-AD42-A7AB-C9A1188FE8E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4961247F-26FC-7140-94BA-5F380292930C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="700" yWindow="460" windowWidth="22680" windowHeight="16540" xr2:uid="{8DD15795-9B77-D142-AB16-8DEEBD71ECC9}"/>
+    <workbookView xWindow="6120" yWindow="460" windowWidth="22680" windowHeight="16540" xr2:uid="{8DD15795-9B77-D142-AB16-8DEEBD71ECC9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="115">
   <si>
     <t>L7</t>
   </si>
@@ -77,12 +77,6 @@
     <t>se</t>
   </si>
   <si>
-    <t>Period</t>
-  </si>
-  <si>
-    <t>Lab no.</t>
-  </si>
-  <si>
     <t xml:space="preserve">1050±40 </t>
   </si>
   <si>
@@ -381,6 +375,9 @@
   </si>
   <si>
     <t>P019</t>
+  </si>
+  <si>
+    <t>Lab code</t>
   </si>
 </sst>
 </file>
@@ -747,28 +744,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C44DE8E0-CB48-C741-8CBC-BBB68EC49E9D}">
-  <dimension ref="A1:L32"/>
+  <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.1640625" customWidth="1"/>
-    <col min="2" max="2" width="11.5" customWidth="1"/>
+    <col min="2" max="2" width="9.5" customWidth="1"/>
     <col min="3" max="3" width="7" customWidth="1"/>
     <col min="4" max="4" width="9.1640625" customWidth="1"/>
     <col min="5" max="5" width="8" customWidth="1"/>
-    <col min="7" max="7" width="26.1640625" customWidth="1"/>
-    <col min="8" max="8" width="10" customWidth="1"/>
-    <col min="9" max="9" width="7.6640625" customWidth="1"/>
-    <col min="10" max="10" width="9.5" customWidth="1"/>
+    <col min="7" max="7" width="24.5" customWidth="1"/>
+    <col min="8" max="8" width="7.6640625" customWidth="1"/>
+    <col min="9" max="9" width="9.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>114</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>7</v>
@@ -789,24 +785,21 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>95</v>
       </c>
       <c r="D2" s="1">
         <v>-130</v>
@@ -815,28 +808,28 @@
         <v>-150</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="H2" s="1">
+        <v>1050</v>
+      </c>
+      <c r="I2" s="1">
+        <v>40</v>
+      </c>
+      <c r="K2" s="2"/>
+    </row>
+    <row r="3" spans="1:11" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="I2" s="1">
-        <v>1050</v>
-      </c>
-      <c r="J2" s="1">
-        <v>40</v>
-      </c>
-      <c r="L2" s="2"/>
-    </row>
-    <row r="3" spans="1:12" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="D3" s="1">
         <v>-20</v>
@@ -845,27 +838,27 @@
         <v>-30</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="H3" s="1">
+        <v>340</v>
+      </c>
+      <c r="I3" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="I3" s="1">
-        <v>340</v>
-      </c>
-      <c r="J3" s="1">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="D4" s="1">
         <v>-150</v>
@@ -874,27 +867,27 @@
         <v>-170</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="H4" s="1">
+        <v>1240</v>
+      </c>
+      <c r="I4" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="I4" s="1">
-        <v>1240</v>
-      </c>
-      <c r="J4" s="1">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="D5" s="1">
         <v>0</v>
@@ -903,21 +896,21 @@
         <v>-10</v>
       </c>
       <c r="F5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="D6" s="1">
         <v>-36</v>
@@ -926,21 +919,21 @@
         <v>-56</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D7" s="1">
         <v>-70</v>
@@ -949,27 +942,27 @@
         <v>-90</v>
       </c>
       <c r="F7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H7" s="1">
+        <v>900</v>
+      </c>
+      <c r="I7" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="I7" s="1">
-        <v>900</v>
-      </c>
-      <c r="J7" s="1">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="D8" s="1">
         <v>-70</v>
@@ -978,21 +971,21 @@
         <v>-90</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D9" s="1">
         <v>-25</v>
@@ -1001,27 +994,27 @@
         <v>-45</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
+      </c>
+      <c r="H9" s="1">
+        <v>250</v>
       </c>
       <c r="I9" s="1">
-        <v>250</v>
-      </c>
-      <c r="J9" s="1">
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:12" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D10" s="1">
         <v>-44</v>
@@ -1030,27 +1023,27 @@
         <v>-80</v>
       </c>
       <c r="F10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="H10" s="1">
+        <v>270</v>
+      </c>
+      <c r="I10" s="1">
         <v>40</v>
       </c>
-      <c r="G10" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="I10" s="1">
-        <v>270</v>
-      </c>
-      <c r="J10" s="1">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:11" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D11" s="1">
         <v>-30</v>
@@ -1059,21 +1052,21 @@
         <v>-70</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D12" s="1">
         <v>4</v>
@@ -1082,21 +1075,21 @@
         <v>-56</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
+      </c>
+      <c r="H12" s="1">
+        <v>510</v>
       </c>
       <c r="I12" s="1">
-        <v>510</v>
-      </c>
-      <c r="J12" s="1">
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:12" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>5</v>
@@ -1111,15 +1104,15 @@
         <v>-70</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>2</v>
@@ -1134,21 +1127,21 @@
         <v>-60</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
+      </c>
+      <c r="H14" s="1">
+        <v>600</v>
       </c>
       <c r="I14" s="1">
-        <v>600</v>
-      </c>
-      <c r="J14" s="1">
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:12" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>5</v>
@@ -1163,21 +1156,21 @@
         <v>-30</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D16" s="1">
         <v>-28</v>
@@ -1186,27 +1179,27 @@
         <v>-70</v>
       </c>
       <c r="F16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H16" s="1">
+        <v>360</v>
+      </c>
+      <c r="I16" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="I16" s="1">
-        <v>360</v>
-      </c>
-      <c r="J16" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>50</v>
       </c>
       <c r="D17" s="1">
         <v>-110</v>
@@ -1215,27 +1208,27 @@
         <v>-130</v>
       </c>
       <c r="F17" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="H17" s="1">
+        <v>310</v>
+      </c>
+      <c r="I17" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="G17" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="I17" s="1">
-        <v>310</v>
-      </c>
-      <c r="J17" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="D18" s="1">
         <v>-100</v>
@@ -1244,27 +1237,27 @@
         <v>-120</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
+      </c>
+      <c r="H18" s="1">
+        <v>800</v>
       </c>
       <c r="I18" s="1">
-        <v>800</v>
-      </c>
-      <c r="J18" s="1">
         <v>120</v>
       </c>
     </row>
-    <row r="19" spans="1:10" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D19" s="1">
         <v>-100</v>
@@ -1273,27 +1266,27 @@
         <v>-120</v>
       </c>
       <c r="F19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="H19" s="1">
+        <v>1190</v>
+      </c>
+      <c r="I19" s="1">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="G19" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="I19" s="1">
-        <v>1190</v>
-      </c>
-      <c r="J19" s="1">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="D20" s="1">
         <v>10</v>
@@ -1302,27 +1295,27 @@
         <v>-10</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
+      </c>
+      <c r="H20" s="1">
+        <v>920</v>
       </c>
       <c r="I20" s="1">
-        <v>920</v>
-      </c>
-      <c r="J20" s="1">
         <v>105</v>
       </c>
     </row>
-    <row r="21" spans="1:10" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D21" s="1">
         <v>6</v>
@@ -1331,27 +1324,27 @@
         <v>-51</v>
       </c>
       <c r="F21" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="H21" s="1">
+        <v>340</v>
+      </c>
+      <c r="I21" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="I21" s="1">
-        <v>340</v>
-      </c>
-      <c r="J21" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="D22" s="1">
         <v>-180</v>
@@ -1360,24 +1353,24 @@
         <v>-190</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
+      </c>
+      <c r="H22" s="1">
+        <v>1870</v>
       </c>
       <c r="I22" s="1">
-        <v>1870</v>
-      </c>
-      <c r="J22" s="1">
         <v>110</v>
       </c>
     </row>
-    <row r="23" spans="1:10" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>3</v>
@@ -1389,21 +1382,21 @@
         <v>-40</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D24" s="1">
         <v>20</v>
@@ -1412,21 +1405,21 @@
         <v>-57</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D25" s="1">
         <v>-10</v>
@@ -1435,27 +1428,27 @@
         <v>-110</v>
       </c>
       <c r="F25" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H25" s="1">
+        <v>280</v>
+      </c>
+      <c r="I25" s="1">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="G25" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="I25" s="1">
-        <v>280</v>
-      </c>
-      <c r="J25" s="1">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="C26" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D26" s="1">
         <v>-160</v>
@@ -1464,27 +1457,27 @@
         <v>-180</v>
       </c>
       <c r="F26" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="H26" s="1">
+        <v>920</v>
+      </c>
+      <c r="I26" s="1">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="G26" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="I26" s="1">
-        <v>920</v>
-      </c>
-      <c r="J26" s="1">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>76</v>
-      </c>
       <c r="C27" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D27" s="1">
         <v>-70</v>
@@ -1493,27 +1486,27 @@
         <v>-90</v>
       </c>
       <c r="F27" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="H27" s="1">
+        <v>1030</v>
+      </c>
+      <c r="I27" s="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="G27" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="I27" s="1">
-        <v>1030</v>
-      </c>
-      <c r="J27" s="1">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>79</v>
-      </c>
       <c r="C28" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D28" s="1">
         <v>-10</v>
@@ -1522,27 +1515,27 @@
         <v>-30</v>
       </c>
       <c r="F28" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="H28" s="1">
+        <v>610</v>
+      </c>
+      <c r="I28" s="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="G28" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="I28" s="1">
-        <v>610</v>
-      </c>
-      <c r="J28" s="1">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+      <c r="C29" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>83</v>
       </c>
       <c r="D29" s="1">
         <v>-160</v>
@@ -1551,27 +1544,27 @@
         <v>-180</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
+      </c>
+      <c r="H29" s="1">
+        <v>1170</v>
       </c>
       <c r="I29" s="1">
-        <v>1170</v>
-      </c>
-      <c r="J29" s="1">
         <v>70</v>
       </c>
     </row>
-    <row r="30" spans="1:10" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D30" s="1">
         <v>-170</v>
@@ -1580,27 +1573,27 @@
         <v>-180</v>
       </c>
       <c r="F30" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="H30" s="1">
+        <v>1080</v>
+      </c>
+      <c r="I30" s="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="G30" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="I30" s="1">
-        <v>1080</v>
-      </c>
-      <c r="J30" s="1">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+      <c r="C31" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="D31" s="1">
         <v>-130</v>
@@ -1609,27 +1602,27 @@
         <v>-150</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
+      </c>
+      <c r="H31" s="1">
+        <v>1020</v>
       </c>
       <c r="I31" s="1">
-        <v>1020</v>
-      </c>
-      <c r="J31" s="1">
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="1:10" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D32" s="1">
         <v>-130</v>
@@ -1638,15 +1631,15 @@
         <v>-150</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
+      </c>
+      <c r="H32" s="1">
+        <v>1480</v>
       </c>
       <c r="I32" s="1">
-        <v>1480</v>
-      </c>
-      <c r="J32" s="1">
         <v>70</v>
       </c>
     </row>

</xml_diff>

<commit_message>
change texts in the datafile and the caption in the code
</commit_message>
<xml_diff>
--- a/analysis/data/raw_data/KWL_C14_dates.xlsx
+++ b/analysis/data/raw_data/KWL_C14_dates.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/EmilyWang/Desktop/School document/LW-Paper/kwl-ornaments-2019/analysis/data/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4961247F-26FC-7140-94BA-5F380292930C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3809D389-5AFB-9942-83D0-9C1E2AB71960}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6120" yWindow="460" windowWidth="22680" windowHeight="16540" xr2:uid="{8DD15795-9B77-D142-AB16-8DEEBD71ECC9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -53,9 +54,6 @@
     <t>P089</t>
   </si>
   <si>
-    <t>Details</t>
-  </si>
-  <si>
     <t>Square</t>
   </si>
   <si>
@@ -338,39 +336,12 @@
     <t>sterile deposit</t>
   </si>
   <si>
-    <t>midden 44</t>
-  </si>
-  <si>
-    <t>midden 193</t>
-  </si>
-  <si>
     <t>P168</t>
   </si>
   <si>
     <t>L1</t>
   </si>
   <si>
-    <t>midden 26</t>
-  </si>
-  <si>
-    <t>midden 172</t>
-  </si>
-  <si>
-    <t>burial 66</t>
-  </si>
-  <si>
-    <t>burial 30</t>
-  </si>
-  <si>
-    <t>burial 9</t>
-  </si>
-  <si>
-    <t>burial 20</t>
-  </si>
-  <si>
-    <t>burial 95</t>
-  </si>
-  <si>
     <t>P018</t>
   </si>
   <si>
@@ -378,6 +349,36 @@
   </si>
   <si>
     <t>Lab code</t>
+  </si>
+  <si>
+    <t>Context</t>
+  </si>
+  <si>
+    <t>burial, M020</t>
+  </si>
+  <si>
+    <t>midden, H044</t>
+  </si>
+  <si>
+    <t>burial, M009</t>
+  </si>
+  <si>
+    <t>burial, M039</t>
+  </si>
+  <si>
+    <t>burial, M066</t>
+  </si>
+  <si>
+    <t>midden, H193</t>
+  </si>
+  <si>
+    <t>midden, H026</t>
+  </si>
+  <si>
+    <t>burial, M095</t>
+  </si>
+  <si>
+    <t>midden H172</t>
   </si>
 </sst>
 </file>
@@ -746,8 +747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C44DE8E0-CB48-C741-8CBC-BBB68EC49E9D}">
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -757,49 +758,49 @@
     <col min="3" max="3" width="7" customWidth="1"/>
     <col min="4" max="4" width="9.1640625" customWidth="1"/>
     <col min="5" max="5" width="8" customWidth="1"/>
-    <col min="7" max="7" width="24.5" customWidth="1"/>
-    <col min="8" max="8" width="7.6640625" customWidth="1"/>
-    <col min="9" max="9" width="9.5" customWidth="1"/>
+    <col min="7" max="7" width="7.6640625" customWidth="1"/>
+    <col min="8" max="8" width="9.5" customWidth="1"/>
+    <col min="9" max="9" width="24.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>13</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>93</v>
       </c>
       <c r="D2" s="1">
         <v>-130</v>
@@ -808,28 +809,28 @@
         <v>-150</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>99</v>
+        <v>13</v>
+      </c>
+      <c r="G2" s="1">
+        <v>1050</v>
       </c>
       <c r="H2" s="1">
-        <v>1050</v>
-      </c>
-      <c r="I2" s="1">
         <v>40</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>98</v>
       </c>
       <c r="K2" s="2"/>
     </row>
     <row r="3" spans="1:11" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="D3" s="1">
         <v>-20</v>
@@ -838,27 +839,27 @@
         <v>-30</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>99</v>
+        <v>17</v>
+      </c>
+      <c r="G3" s="1">
+        <v>340</v>
       </c>
       <c r="H3" s="1">
-        <v>340</v>
-      </c>
-      <c r="I3" s="1">
         <v>30</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="D4" s="1">
         <v>-150</v>
@@ -867,27 +868,27 @@
         <v>-170</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>99</v>
+        <v>21</v>
+      </c>
+      <c r="G4" s="1">
+        <v>1240</v>
       </c>
       <c r="H4" s="1">
-        <v>1240</v>
-      </c>
-      <c r="I4" s="1">
         <v>30</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:11" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="D5" s="1">
         <v>0</v>
@@ -896,21 +897,21 @@
         <v>-10</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>99</v>
+        <v>25</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:11" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="D6" s="1">
         <v>-36</v>
@@ -919,21 +920,21 @@
         <v>-56</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>100</v>
+        <v>25</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:11" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="D7" s="1">
         <v>-70</v>
@@ -942,27 +943,27 @@
         <v>-90</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>100</v>
+        <v>31</v>
+      </c>
+      <c r="G7" s="1">
+        <v>900</v>
       </c>
       <c r="H7" s="1">
-        <v>900</v>
-      </c>
-      <c r="I7" s="1">
         <v>50</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:11" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="D8" s="1">
         <v>-70</v>
@@ -971,21 +972,21 @@
         <v>-90</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>100</v>
+        <v>25</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:11" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D9" s="1">
         <v>-25</v>
@@ -994,27 +995,27 @@
         <v>-45</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>99</v>
+        <v>35</v>
+      </c>
+      <c r="G9" s="1">
+        <v>250</v>
       </c>
       <c r="H9" s="1">
-        <v>250</v>
-      </c>
-      <c r="I9" s="1">
         <v>40</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="10" spans="1:11" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D10" s="1">
         <v>-44</v>
@@ -1023,27 +1024,27 @@
         <v>-80</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>110</v>
+        <v>37</v>
+      </c>
+      <c r="G10" s="1">
+        <v>270</v>
       </c>
       <c r="H10" s="1">
-        <v>270</v>
-      </c>
-      <c r="I10" s="1">
         <v>40</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:11" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D11" s="1">
         <v>-30</v>
@@ -1052,21 +1053,21 @@
         <v>-70</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>101</v>
+        <v>25</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:11" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="D12" s="1">
         <v>4</v>
@@ -1075,21 +1076,21 @@
         <v>-56</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>109</v>
+        <v>42</v>
+      </c>
+      <c r="G12" s="1">
+        <v>510</v>
       </c>
       <c r="H12" s="1">
-        <v>510</v>
-      </c>
-      <c r="I12" s="1">
         <v>75</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="13" spans="1:11" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>5</v>
@@ -1104,15 +1105,15 @@
         <v>-70</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>99</v>
+        <v>94</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:11" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>2</v>
@@ -1127,21 +1128,21 @@
         <v>-60</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
+      </c>
+      <c r="G14" s="1">
+        <v>600</v>
       </c>
       <c r="H14" s="1">
-        <v>600</v>
-      </c>
-      <c r="I14" s="1">
         <v>75</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:11" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>5</v>
@@ -1156,21 +1157,21 @@
         <v>-30</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>99</v>
+        <v>25</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:11" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="D16" s="1">
         <v>-28</v>
@@ -1179,27 +1180,27 @@
         <v>-70</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>108</v>
+        <v>45</v>
+      </c>
+      <c r="G16" s="1">
+        <v>360</v>
       </c>
       <c r="H16" s="1">
-        <v>360</v>
-      </c>
-      <c r="I16" s="1">
         <v>100</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="D17" s="1">
         <v>-110</v>
@@ -1208,27 +1209,27 @@
         <v>-130</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>99</v>
+        <v>48</v>
+      </c>
+      <c r="G17" s="1">
+        <v>310</v>
       </c>
       <c r="H17" s="1">
-        <v>310</v>
-      </c>
-      <c r="I17" s="1">
         <v>100</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="18" spans="1:9" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="D18" s="1">
         <v>-100</v>
@@ -1237,27 +1238,27 @@
         <v>-120</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>99</v>
+        <v>52</v>
+      </c>
+      <c r="G18" s="1">
+        <v>800</v>
       </c>
       <c r="H18" s="1">
-        <v>800</v>
-      </c>
-      <c r="I18" s="1">
         <v>120</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="19" spans="1:9" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D19" s="1">
         <v>-100</v>
@@ -1266,27 +1267,27 @@
         <v>-120</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>107</v>
+        <v>54</v>
+      </c>
+      <c r="G19" s="1">
+        <v>1190</v>
       </c>
       <c r="H19" s="1">
-        <v>1190</v>
-      </c>
-      <c r="I19" s="1">
         <v>70</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="20" spans="1:9" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="D20" s="1">
         <v>10</v>
@@ -1295,27 +1296,27 @@
         <v>-10</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>99</v>
+        <v>58</v>
+      </c>
+      <c r="G20" s="1">
+        <v>920</v>
       </c>
       <c r="H20" s="1">
-        <v>920</v>
-      </c>
-      <c r="I20" s="1">
         <v>105</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="21" spans="1:9" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D21" s="1">
         <v>6</v>
@@ -1324,27 +1325,27 @@
         <v>-51</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>102</v>
+        <v>60</v>
+      </c>
+      <c r="G21" s="1">
+        <v>340</v>
       </c>
       <c r="H21" s="1">
-        <v>340</v>
-      </c>
-      <c r="I21" s="1">
         <v>100</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="22" spans="1:9" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="D22" s="1">
         <v>-180</v>
@@ -1353,24 +1354,24 @@
         <v>-190</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>99</v>
+        <v>63</v>
+      </c>
+      <c r="G22" s="1">
+        <v>1870</v>
       </c>
       <c r="H22" s="1">
-        <v>1870</v>
-      </c>
-      <c r="I22" s="1">
         <v>110</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="23" spans="1:9" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>3</v>
@@ -1382,21 +1383,21 @@
         <v>-40</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>105</v>
+        <v>25</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="24" spans="1:9" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D24" s="1">
         <v>20</v>
@@ -1405,21 +1406,21 @@
         <v>-57</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>111</v>
+        <v>25</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="25" spans="1:9" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D25" s="1">
         <v>-10</v>
@@ -1428,27 +1429,27 @@
         <v>-110</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>106</v>
+        <v>68</v>
+      </c>
+      <c r="G25" s="1">
+        <v>280</v>
       </c>
       <c r="H25" s="1">
-        <v>280</v>
-      </c>
-      <c r="I25" s="1">
         <v>70</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="26" spans="1:9" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="C26" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D26" s="1">
         <v>-160</v>
@@ -1457,27 +1458,27 @@
         <v>-180</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>99</v>
+        <v>71</v>
+      </c>
+      <c r="G26" s="1">
+        <v>920</v>
       </c>
       <c r="H26" s="1">
-        <v>920</v>
-      </c>
-      <c r="I26" s="1">
         <v>70</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="27" spans="1:9" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>74</v>
-      </c>
       <c r="C27" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D27" s="1">
         <v>-70</v>
@@ -1486,27 +1487,27 @@
         <v>-90</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>99</v>
+        <v>74</v>
+      </c>
+      <c r="G27" s="1">
+        <v>1030</v>
       </c>
       <c r="H27" s="1">
-        <v>1030</v>
-      </c>
-      <c r="I27" s="1">
         <v>80</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="28" spans="1:9" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>77</v>
-      </c>
       <c r="C28" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D28" s="1">
         <v>-10</v>
@@ -1515,27 +1516,27 @@
         <v>-30</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>99</v>
+        <v>77</v>
+      </c>
+      <c r="G28" s="1">
+        <v>610</v>
       </c>
       <c r="H28" s="1">
-        <v>610</v>
-      </c>
-      <c r="I28" s="1">
         <v>90</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="29" spans="1:9" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="C29" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>81</v>
       </c>
       <c r="D29" s="1">
         <v>-160</v>
@@ -1544,27 +1545,27 @@
         <v>-180</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>99</v>
+        <v>81</v>
+      </c>
+      <c r="G29" s="1">
+        <v>1170</v>
       </c>
       <c r="H29" s="1">
-        <v>1170</v>
-      </c>
-      <c r="I29" s="1">
         <v>70</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="30" spans="1:9" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D30" s="1">
         <v>-170</v>
@@ -1573,27 +1574,27 @@
         <v>-180</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>99</v>
+        <v>83</v>
+      </c>
+      <c r="G30" s="1">
+        <v>1080</v>
       </c>
       <c r="H30" s="1">
-        <v>1080</v>
-      </c>
-      <c r="I30" s="1">
         <v>90</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="31" spans="1:9" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="C31" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>87</v>
       </c>
       <c r="D31" s="1">
         <v>-130</v>
@@ -1602,27 +1603,27 @@
         <v>-150</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>100</v>
+        <v>87</v>
+      </c>
+      <c r="G31" s="1">
+        <v>1020</v>
       </c>
       <c r="H31" s="1">
-        <v>1020</v>
-      </c>
-      <c r="I31" s="1">
         <v>60</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="32" spans="1:9" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D32" s="1">
         <v>-130</v>
@@ -1631,19 +1632,33 @@
         <v>-150</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>99</v>
+        <v>89</v>
+      </c>
+      <c r="G32" s="1">
+        <v>1480</v>
       </c>
       <c r="H32" s="1">
-        <v>1480</v>
-      </c>
-      <c r="I32" s="1">
         <v>70</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95184E50-A8A2-3348-A325-A464439CC36A}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
removed comma in the C14 data file, and added code in the script file
</commit_message>
<xml_diff>
--- a/analysis/data/raw_data/KWL_C14_dates.xlsx
+++ b/analysis/data/raw_data/KWL_C14_dates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/EmilyWang/Desktop/School document/LW-Paper/kwl-ornaments-2019/analysis/data/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3809D389-5AFB-9942-83D0-9C1E2AB71960}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA99184B-993B-9445-A77D-9B791B0BE075}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6120" yWindow="460" windowWidth="22680" windowHeight="16540" xr2:uid="{8DD15795-9B77-D142-AB16-8DEEBD71ECC9}"/>
   </bookViews>
@@ -354,31 +354,31 @@
     <t>Context</t>
   </si>
   <si>
-    <t>burial, M020</t>
-  </si>
-  <si>
-    <t>midden, H044</t>
-  </si>
-  <si>
-    <t>burial, M009</t>
-  </si>
-  <si>
-    <t>burial, M039</t>
-  </si>
-  <si>
-    <t>burial, M066</t>
-  </si>
-  <si>
-    <t>midden, H193</t>
-  </si>
-  <si>
-    <t>midden, H026</t>
-  </si>
-  <si>
-    <t>burial, M095</t>
-  </si>
-  <si>
     <t>midden H172</t>
+  </si>
+  <si>
+    <t>burial M020</t>
+  </si>
+  <si>
+    <t>midden H044</t>
+  </si>
+  <si>
+    <t>burial M009</t>
+  </si>
+  <si>
+    <t>burial M039</t>
+  </si>
+  <si>
+    <t>burial M066</t>
+  </si>
+  <si>
+    <t>midden H193</t>
+  </si>
+  <si>
+    <t>midden H026</t>
+  </si>
+  <si>
+    <t>burial M095</t>
   </si>
 </sst>
 </file>
@@ -748,7 +748,7 @@
   <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1033,7 +1033,7 @@
         <v>40</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="11" spans="1:11" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
@@ -1056,7 +1056,7 @@
         <v>25</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12" spans="1:11" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
@@ -1085,7 +1085,7 @@
         <v>75</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:11" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
@@ -1189,7 +1189,7 @@
         <v>100</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
@@ -1276,7 +1276,7 @@
         <v>70</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="20" spans="1:9" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
@@ -1334,7 +1334,7 @@
         <v>100</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="22" spans="1:9" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
@@ -1386,7 +1386,7 @@
         <v>25</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="24" spans="1:9" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
@@ -1409,7 +1409,7 @@
         <v>25</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="25" spans="1:9" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
@@ -1438,7 +1438,7 @@
         <v>70</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
     </row>
     <row r="26" spans="1:9" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updates to C14 table
</commit_message>
<xml_diff>
--- a/analysis/data/raw_data/KWL_C14_dates.xlsx
+++ b/analysis/data/raw_data/KWL_C14_dates.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/EmilyWang/Desktop/School document/LW-Paper/kwl-ornaments-2019/analysis/data/raw_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bmarwick/Desktop/kwl-ornaments/analysis/data/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA99184B-993B-9445-A77D-9B791B0BE075}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D989DF8A-EFDF-0B4D-8DD3-2721E58EE9C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6120" yWindow="460" windowWidth="22680" windowHeight="16540" xr2:uid="{8DD15795-9B77-D142-AB16-8DEEBD71ECC9}"/>
   </bookViews>
@@ -24,9 +24,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -354,31 +352,31 @@
     <t>Context</t>
   </si>
   <si>
+    <t>burial, M020</t>
+  </si>
+  <si>
+    <t>midden, H044</t>
+  </si>
+  <si>
+    <t>burial, M009</t>
+  </si>
+  <si>
+    <t>burial, M039</t>
+  </si>
+  <si>
+    <t>burial, M066</t>
+  </si>
+  <si>
+    <t>midden, H193</t>
+  </si>
+  <si>
+    <t>midden, H026</t>
+  </si>
+  <si>
+    <t>burial, M095</t>
+  </si>
+  <si>
     <t>midden H172</t>
-  </si>
-  <si>
-    <t>burial M020</t>
-  </si>
-  <si>
-    <t>midden H044</t>
-  </si>
-  <si>
-    <t>burial M009</t>
-  </si>
-  <si>
-    <t>burial M039</t>
-  </si>
-  <si>
-    <t>burial M066</t>
-  </si>
-  <si>
-    <t>midden H193</t>
-  </si>
-  <si>
-    <t>midden H026</t>
-  </si>
-  <si>
-    <t>burial M095</t>
   </si>
 </sst>
 </file>
@@ -747,8 +745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C44DE8E0-CB48-C741-8CBC-BBB68EC49E9D}">
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1033,7 +1031,7 @@
         <v>40</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:11" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
@@ -1056,7 +1054,7 @@
         <v>25</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:11" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
@@ -1085,7 +1083,7 @@
         <v>75</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="13" spans="1:11" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
@@ -1189,7 +1187,7 @@
         <v>100</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
@@ -1276,7 +1274,7 @@
         <v>70</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="20" spans="1:9" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
@@ -1334,7 +1332,7 @@
         <v>100</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="22" spans="1:9" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
@@ -1386,7 +1384,7 @@
         <v>25</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="24" spans="1:9" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
@@ -1409,7 +1407,7 @@
         <v>25</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="25" spans="1:9" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
@@ -1438,7 +1436,7 @@
         <v>70</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
     </row>
     <row r="26" spans="1:9" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
update C14 data file and the caption in the code
</commit_message>
<xml_diff>
--- a/analysis/data/raw_data/KWL_C14_dates.xlsx
+++ b/analysis/data/raw_data/KWL_C14_dates.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bmarwick/Desktop/kwl-ornaments/analysis/data/raw_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/EmilyWang/Desktop/School document/LW-Paper/kwl-ornaments-2019/analysis/data/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D989DF8A-EFDF-0B4D-8DD3-2721E58EE9C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{705C41F7-85AD-4644-8365-7B4A95993335}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6120" yWindow="460" windowWidth="22680" windowHeight="16540" xr2:uid="{8DD15795-9B77-D142-AB16-8DEEBD71ECC9}"/>
   </bookViews>
@@ -24,7 +24,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -352,31 +354,31 @@
     <t>Context</t>
   </si>
   <si>
-    <t>burial, M020</t>
-  </si>
-  <si>
-    <t>midden, H044</t>
-  </si>
-  <si>
-    <t>burial, M009</t>
-  </si>
-  <si>
-    <t>burial, M039</t>
-  </si>
-  <si>
-    <t>burial, M066</t>
-  </si>
-  <si>
-    <t>midden, H193</t>
-  </si>
-  <si>
-    <t>midden, H026</t>
-  </si>
-  <si>
-    <t>burial, M095</t>
-  </si>
-  <si>
     <t>midden H172</t>
+  </si>
+  <si>
+    <t>burial M020</t>
+  </si>
+  <si>
+    <t>midden H044</t>
+  </si>
+  <si>
+    <t>burial M009</t>
+  </si>
+  <si>
+    <t>burial M039</t>
+  </si>
+  <si>
+    <t>burial M066</t>
+  </si>
+  <si>
+    <t>midden H193</t>
+  </si>
+  <si>
+    <t>midden H026</t>
+  </si>
+  <si>
+    <t>burial M095</t>
   </si>
 </sst>
 </file>
@@ -745,8 +747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C44DE8E0-CB48-C741-8CBC-BBB68EC49E9D}">
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1031,7 +1033,7 @@
         <v>40</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="11" spans="1:11" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
@@ -1054,7 +1056,7 @@
         <v>25</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12" spans="1:11" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
@@ -1083,7 +1085,7 @@
         <v>75</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:11" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
@@ -1187,7 +1189,7 @@
         <v>100</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
@@ -1274,7 +1276,7 @@
         <v>70</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="20" spans="1:9" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
@@ -1332,7 +1334,7 @@
         <v>100</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="22" spans="1:9" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
@@ -1384,7 +1386,7 @@
         <v>25</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="24" spans="1:9" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
@@ -1407,7 +1409,7 @@
         <v>25</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="25" spans="1:9" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">
@@ -1436,7 +1438,7 @@
         <v>70</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
     </row>
     <row r="26" spans="1:9" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.25">

</xml_diff>